<commit_message>
loading and cau template
</commit_message>
<xml_diff>
--- a/table_1.xlsx
+++ b/table_1.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,103 +422,611 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr"/>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Data</t>
+        </is>
+      </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>IoU mask</t>
+          <t>Methods</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>IoU vect.</t>
+          <t>Argument Mining</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Argument Pair Extraction</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>B [8]</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>0.74</t>
-        </is>
-      </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.53</t>
+          <t>Pre.</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Rec.</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>F1</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Pre.</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Rec.</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>F1</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>B + C</t>
+          <t>RR-Submission-v2</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0.79</t>
+          <t>PL-H-LSTM-CRF</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.58</t>
+          <t>67.02</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>68.49</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>67.75</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>19.74</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>19.13</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>19.43</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>B + C + OV</t>
-        </is>
-      </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0.79</t>
+          <t>MT-H-LSTM-CRF</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.78</t>
+          <t>70.74</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>69.46</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>70.09</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>27.24</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>26.00</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>26.61</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Ours</t>
-        </is>
-      </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>0.81</t>
+          <t>MLMC</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.8</t>
+          <t>69.53</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>73.27</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>71.35</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>37.15</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>29.38</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>32.81</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>MRC-APE-Bert</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>73.36</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>68.35</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>70.77</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>42.26</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>34.06</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>37.72</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>MRC-APE-Sep.</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>72.45</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>71.58</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>72.01</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>41.09</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>36.99</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>38.93</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>MRC-APE (Ours)</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>71.83</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>73.05</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>72.43</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>41.83</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>38.17</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>39.92</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>RR-Passage-v1</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>PL-H-LSTM-CRF</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>73.10</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>67.65</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>70.27</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>21.24</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>19.30</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>20.22</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>MT-H-LSTM-CRF</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>71.85</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>71.01</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>71.43</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>30.08</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>29.55</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>29.81</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>MLMC</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>66.79</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>72.17</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>69.38</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>40.27</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>29.53</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>34.07</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>MRC-APE-Bert</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>66.81</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>69.84</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>68.29</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>34.70</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>35.53</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>35.11</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>MRC-APE-Sep.</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>75.27</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>67.90</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>71.39</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>36.63</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>40.05</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>38.26</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>MRC-APE (Ours)</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>76.39</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>70.62</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>73.39</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>37.70</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>44.00</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>40.61</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="96">
+    <mergeCell ref="D12"/>
+    <mergeCell ref="D9"/>
+    <mergeCell ref="F9"/>
+    <mergeCell ref="H3"/>
+    <mergeCell ref="C7"/>
+    <mergeCell ref="B6"/>
+    <mergeCell ref="E7"/>
+    <mergeCell ref="D14"/>
+    <mergeCell ref="F14"/>
+    <mergeCell ref="H5"/>
+    <mergeCell ref="B4"/>
+    <mergeCell ref="G2"/>
+    <mergeCell ref="H4"/>
+    <mergeCell ref="F12"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="H6"/>
+    <mergeCell ref="G6"/>
+    <mergeCell ref="C9"/>
+    <mergeCell ref="B8"/>
+    <mergeCell ref="E9"/>
+    <mergeCell ref="A3"/>
+    <mergeCell ref="E6"/>
+    <mergeCell ref="H7"/>
+    <mergeCell ref="C11"/>
+    <mergeCell ref="B10"/>
+    <mergeCell ref="E11"/>
+    <mergeCell ref="G14"/>
+    <mergeCell ref="B9"/>
+    <mergeCell ref="D3"/>
+    <mergeCell ref="G4"/>
+    <mergeCell ref="B5"/>
+    <mergeCell ref="D5"/>
+    <mergeCell ref="C13"/>
+    <mergeCell ref="F11"/>
+    <mergeCell ref="E8"/>
+    <mergeCell ref="H9"/>
+    <mergeCell ref="G8"/>
+    <mergeCell ref="B12"/>
+    <mergeCell ref="F3"/>
+    <mergeCell ref="C10"/>
+    <mergeCell ref="E10"/>
+    <mergeCell ref="G10"/>
+    <mergeCell ref="B14"/>
     <mergeCell ref="B1"/>
-    <mergeCell ref="B4"/>
-    <mergeCell ref="A5"/>
+    <mergeCell ref="B13"/>
+    <mergeCell ref="G3"/>
+    <mergeCell ref="D7"/>
+    <mergeCell ref="C2"/>
+    <mergeCell ref="E2"/>
+    <mergeCell ref="G5"/>
+    <mergeCell ref="F13"/>
+    <mergeCell ref="H13"/>
+    <mergeCell ref="D8"/>
+    <mergeCell ref="H8"/>
+    <mergeCell ref="E12"/>
+    <mergeCell ref="G12"/>
+    <mergeCell ref="C6"/>
+    <mergeCell ref="H10"/>
+    <mergeCell ref="F6"/>
+    <mergeCell ref="C14"/>
+    <mergeCell ref="E14"/>
     <mergeCell ref="C4"/>
-    <mergeCell ref="A4"/>
+    <mergeCell ref="E4"/>
+    <mergeCell ref="D6"/>
+    <mergeCell ref="G7"/>
+    <mergeCell ref="B11"/>
+    <mergeCell ref="D11"/>
+    <mergeCell ref="D13"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="D4"/>
+    <mergeCell ref="C8"/>
+    <mergeCell ref="H12"/>
+    <mergeCell ref="H14"/>
+    <mergeCell ref="G9"/>
+    <mergeCell ref="A9"/>
     <mergeCell ref="C3"/>
-    <mergeCell ref="A3"/>
-    <mergeCell ref="C1"/>
-    <mergeCell ref="B2"/>
-    <mergeCell ref="A2"/>
-    <mergeCell ref="C2"/>
+    <mergeCell ref="F4"/>
+    <mergeCell ref="E3"/>
+    <mergeCell ref="B7"/>
+    <mergeCell ref="D10"/>
+    <mergeCell ref="G11"/>
+    <mergeCell ref="F10"/>
     <mergeCell ref="B3"/>
-    <mergeCell ref="B5"/>
     <mergeCell ref="C5"/>
     <mergeCell ref="A1"/>
+    <mergeCell ref="E5"/>
+    <mergeCell ref="F7"/>
+    <mergeCell ref="D2"/>
+    <mergeCell ref="F5"/>
+    <mergeCell ref="E13"/>
+    <mergeCell ref="G13"/>
+    <mergeCell ref="F8"/>
+    <mergeCell ref="F2"/>
+    <mergeCell ref="C12"/>
+    <mergeCell ref="H2"/>
+    <mergeCell ref="H11"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>